<commit_message>
eval stuff moved in
</commit_message>
<xml_diff>
--- a/data/raw/requirements.xlsx
+++ b/data/raw/requirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evie/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/evie/Desktop/l4_final/app/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{11471266-A49E-0B4A-B36F-A6ADC89FF98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73756897-35B3-D743-81F3-BD22D90CC41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,6 +109,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -361,9 +362,9 @@
   </sheetPr>
   <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -372,7 +373,7 @@
     <col min="2" max="2" width="35.1640625" customWidth="1"/>
     <col min="3" max="3" width="34.6640625" customWidth="1"/>
     <col min="4" max="8" width="18.83203125" customWidth="1"/>
-    <col min="9" max="9" width="94.33203125" customWidth="1"/>
+    <col min="9" max="9" width="55.5" customWidth="1"/>
     <col min="10" max="10" width="37.1640625" customWidth="1"/>
     <col min="11" max="13" width="18.83203125" customWidth="1"/>
     <col min="14" max="14" width="90.6640625" customWidth="1"/>
@@ -435,7 +436,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" ht="16">
       <c r="A2" s="2">
         <v>44859.643958333334</v>
       </c>
@@ -482,7 +483,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:18" ht="16">
       <c r="A3" s="2">
         <v>44860.325937499998</v>
       </c>
@@ -529,7 +530,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" ht="16">
       <c r="A4" s="2">
         <v>44860.523425925923</v>
       </c>
@@ -576,7 +577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" ht="16">
       <c r="A5" s="2">
         <v>44861.774444444447</v>
       </c>
@@ -623,7 +624,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" ht="16">
       <c r="A6" s="2">
         <v>44861.928298611114</v>
       </c>
@@ -670,7 +671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" ht="16">
       <c r="A7" s="2">
         <v>44862.832592592589</v>
       </c>
@@ -717,7 +718,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" ht="16">
       <c r="A8" s="2">
         <v>44862.96806712963</v>
       </c>
@@ -764,7 +765,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" ht="16">
       <c r="A9" s="2">
         <v>44863.382372685184</v>
       </c>
@@ -811,7 +812,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" ht="16">
       <c r="A10" s="2">
         <v>44863.908321759256</v>
       </c>
@@ -858,7 +859,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" ht="16">
       <c r="A11" s="2">
         <v>44864.285740740743</v>
       </c>
@@ -905,7 +906,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" ht="16">
       <c r="A12" s="2">
         <v>44864.556990740741</v>
       </c>
@@ -952,7 +953,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" ht="16">
       <c r="A13" s="2">
         <v>44865.087187500001</v>
       </c>

</xml_diff>